<commit_message>
update trang quan ly he thong may
</commit_message>
<xml_diff>
--- a/app/public/data/importStation.xlsx
+++ b/app/public/data/importStation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Works\vldc_2024\vldc\app\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9EF5002-6DFA-414A-A1A8-5146F41FC6AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8F36DD-5B45-48F6-B3A8-0CF34DF3C09F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4635" yWindow="-11640" windowWidth="20730" windowHeight="11310" xr2:uid="{8907BB97-B73E-41CB-8301-7599B5329D29}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2182" uniqueCount="813">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2144" uniqueCount="812">
   <si>
     <t>STT</t>
   </si>
@@ -2461,9 +2461,6 @@
   </si>
   <si>
     <t>CB03</t>
-  </si>
-  <si>
-    <t>15/12/2010</t>
   </si>
 </sst>
 </file>
@@ -2525,7 +2522,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2544,9 +2541,6 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2865,8 +2859,8 @@
   <dimension ref="A1:BI123"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AT1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BI4" sqref="BI4"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="BH2" sqref="BH2:BH43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
@@ -3181,9 +3175,7 @@
       <c r="BG2" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="BH2" s="7" t="s">
-        <v>812</v>
-      </c>
+      <c r="BH2" s="2"/>
     </row>
     <row r="3" spans="1:61" ht="50.4" x14ac:dyDescent="0.3">
       <c r="AB3" s="3" t="s">
@@ -3216,9 +3208,7 @@
       <c r="BG3" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="BH3" s="7" t="s">
-        <v>812</v>
-      </c>
+      <c r="BH3" s="2"/>
     </row>
     <row r="4" spans="1:61" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -3353,9 +3343,7 @@
       <c r="BG4" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="BH4" s="7" t="s">
-        <v>812</v>
-      </c>
+      <c r="BH4" s="2"/>
     </row>
     <row r="5" spans="1:61" ht="50.4" x14ac:dyDescent="0.3">
       <c r="AB5" s="3" t="s">
@@ -3379,9 +3367,7 @@
       <c r="AR5" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="BH5" s="7" t="s">
-        <v>812</v>
-      </c>
+      <c r="BH5" s="2"/>
     </row>
     <row r="6" spans="1:61" ht="84" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -3501,9 +3487,7 @@
       <c r="BG6" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="BH6" s="7" t="s">
-        <v>812</v>
-      </c>
+      <c r="BH6" s="2"/>
     </row>
     <row r="7" spans="1:61" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -3656,9 +3640,7 @@
       <c r="BG7" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="BH7" s="7" t="s">
-        <v>812</v>
-      </c>
+      <c r="BH7" s="2"/>
     </row>
     <row r="8" spans="1:61" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
@@ -3799,9 +3781,7 @@
       <c r="BG8" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="BH8" s="7" t="s">
-        <v>812</v>
-      </c>
+      <c r="BH8" s="2"/>
     </row>
     <row r="9" spans="1:61" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
@@ -3954,9 +3934,7 @@
       <c r="BG9" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="BH9" s="7" t="s">
-        <v>812</v>
-      </c>
+      <c r="BH9" s="2"/>
     </row>
     <row r="10" spans="1:61" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -4103,9 +4081,7 @@
       <c r="BG10" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="BH10" s="7" t="s">
-        <v>812</v>
-      </c>
+      <c r="BH10" s="2"/>
     </row>
     <row r="11" spans="1:61" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
@@ -4240,9 +4216,7 @@
       <c r="BG11" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="BH11" s="7" t="s">
-        <v>812</v>
-      </c>
+      <c r="BH11" s="2"/>
     </row>
     <row r="12" spans="1:61" ht="33.6" x14ac:dyDescent="0.3">
       <c r="AB12" s="3" t="s">
@@ -4260,9 +4234,7 @@
       <c r="AH12" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="BH12" s="7" t="s">
-        <v>812</v>
-      </c>
+      <c r="BH12" s="2"/>
     </row>
     <row r="13" spans="1:61" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
@@ -4427,9 +4399,7 @@
       <c r="BG13" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="BH13" s="7" t="s">
-        <v>812</v>
-      </c>
+      <c r="BH13" s="2"/>
     </row>
     <row r="14" spans="1:61" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
@@ -4570,9 +4540,7 @@
       <c r="BG14" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="BH14" s="7" t="s">
-        <v>812</v>
-      </c>
+      <c r="BH14" s="2"/>
     </row>
     <row r="15" spans="1:61" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
@@ -4716,9 +4684,7 @@
       <c r="BG15" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="BH15" s="7" t="s">
-        <v>812</v>
-      </c>
+      <c r="BH15" s="2"/>
     </row>
     <row r="16" spans="1:61" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
@@ -4865,9 +4831,7 @@
       <c r="BG16" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="BH16" s="7" t="s">
-        <v>812</v>
-      </c>
+      <c r="BH16" s="2"/>
     </row>
     <row r="17" spans="1:60" ht="84" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
@@ -5026,9 +4990,7 @@
       <c r="BG17" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="BH17" s="7" t="s">
-        <v>812</v>
-      </c>
+      <c r="BH17" s="2"/>
     </row>
     <row r="18" spans="1:60" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
@@ -5181,9 +5143,7 @@
       <c r="BG18" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="BH18" s="7" t="s">
-        <v>812</v>
-      </c>
+      <c r="BH18" s="2"/>
     </row>
     <row r="19" spans="1:60" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
@@ -5321,9 +5281,7 @@
       <c r="BG19" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="BH19" s="7" t="s">
-        <v>812</v>
-      </c>
+      <c r="BH19" s="2"/>
     </row>
     <row r="20" spans="1:60" ht="84" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
@@ -5419,9 +5377,7 @@
       <c r="BE20" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="BH20" s="7" t="s">
-        <v>812</v>
-      </c>
+      <c r="BH20" s="2"/>
     </row>
     <row r="21" spans="1:60" ht="50.4" x14ac:dyDescent="0.3">
       <c r="AB21" s="3" t="s">
@@ -5454,9 +5410,7 @@
       <c r="BG21" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="BH21" s="7" t="s">
-        <v>812</v>
-      </c>
+      <c r="BH21" s="2"/>
     </row>
     <row r="22" spans="1:60" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
@@ -5603,9 +5557,7 @@
       <c r="BG22" s="4" t="s">
         <v>403</v>
       </c>
-      <c r="BH22" s="7" t="s">
-        <v>812</v>
-      </c>
+      <c r="BH22" s="2"/>
     </row>
     <row r="23" spans="1:60" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
@@ -5749,9 +5701,7 @@
       <c r="BG23" s="4" t="s">
         <v>419</v>
       </c>
-      <c r="BH23" s="7" t="s">
-        <v>812</v>
-      </c>
+      <c r="BH23" s="2"/>
     </row>
     <row r="24" spans="1:60" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
@@ -5889,9 +5839,7 @@
       <c r="BG24" s="4" t="s">
         <v>435</v>
       </c>
-      <c r="BH24" s="7" t="s">
-        <v>812</v>
-      </c>
+      <c r="BH24" s="2"/>
     </row>
     <row r="25" spans="1:60" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
@@ -6014,9 +5962,7 @@
       <c r="BG25" s="4" t="s">
         <v>450</v>
       </c>
-      <c r="BH25" s="7" t="s">
-        <v>812</v>
-      </c>
+      <c r="BH25" s="2"/>
     </row>
     <row r="26" spans="1:60" ht="50.4" x14ac:dyDescent="0.3">
       <c r="AB26" s="3" t="s">
@@ -6040,9 +5986,7 @@
       <c r="AR26" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="BH26" s="7" t="s">
-        <v>812</v>
-      </c>
+      <c r="BH26" s="2"/>
     </row>
     <row r="27" spans="1:60" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
@@ -6186,9 +6130,7 @@
       <c r="BG27" s="4" t="s">
         <v>466</v>
       </c>
-      <c r="BH27" s="7" t="s">
-        <v>812</v>
-      </c>
+      <c r="BH27" s="2"/>
     </row>
     <row r="28" spans="1:60" ht="67.2" x14ac:dyDescent="0.3">
       <c r="AB28" s="3" t="s">
@@ -6209,9 +6151,7 @@
       <c r="AR28" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="BH28" s="7" t="s">
-        <v>812</v>
-      </c>
+      <c r="BH28" s="2"/>
     </row>
     <row r="29" spans="1:60" ht="84" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
@@ -6346,9 +6286,7 @@
       <c r="BG29" s="4" t="s">
         <v>482</v>
       </c>
-      <c r="BH29" s="7" t="s">
-        <v>812</v>
-      </c>
+      <c r="BH29" s="2"/>
     </row>
     <row r="30" spans="1:60" ht="50.4" x14ac:dyDescent="0.3">
       <c r="AB30" s="3" t="s">
@@ -6378,9 +6316,7 @@
       <c r="AR30" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="BH30" s="7" t="s">
-        <v>812</v>
-      </c>
+      <c r="BH30" s="2"/>
     </row>
     <row r="31" spans="1:60" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
@@ -6527,9 +6463,7 @@
       <c r="BG31" s="4" t="s">
         <v>498</v>
       </c>
-      <c r="BH31" s="7" t="s">
-        <v>812</v>
-      </c>
+      <c r="BH31" s="2"/>
     </row>
     <row r="32" spans="1:60" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
@@ -6673,9 +6607,7 @@
       <c r="BG32" s="4" t="s">
         <v>515</v>
       </c>
-      <c r="BH32" s="7" t="s">
-        <v>812</v>
-      </c>
+      <c r="BH32" s="2"/>
     </row>
     <row r="33" spans="1:60" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
@@ -6819,9 +6751,7 @@
       <c r="BG33" s="4" t="s">
         <v>531</v>
       </c>
-      <c r="BH33" s="7" t="s">
-        <v>812</v>
-      </c>
+      <c r="BH33" s="2"/>
     </row>
     <row r="34" spans="1:60" ht="67.2" x14ac:dyDescent="0.3">
       <c r="AB34" s="3" t="s">
@@ -6848,9 +6778,7 @@
       <c r="AR34" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="BH34" s="7" t="s">
-        <v>812</v>
-      </c>
+      <c r="BH34" s="2"/>
     </row>
     <row r="35" spans="1:60" ht="84" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
@@ -6994,9 +6922,7 @@
       <c r="BG35" s="4" t="s">
         <v>545</v>
       </c>
-      <c r="BH35" s="7" t="s">
-        <v>812</v>
-      </c>
+      <c r="BH35" s="2"/>
     </row>
     <row r="36" spans="1:60" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
@@ -7149,9 +7075,7 @@
       <c r="BG36" s="4" t="s">
         <v>560</v>
       </c>
-      <c r="BH36" s="7" t="s">
-        <v>812</v>
-      </c>
+      <c r="BH36" s="2"/>
     </row>
     <row r="37" spans="1:60" ht="67.2" x14ac:dyDescent="0.3">
       <c r="AB37" s="3" t="s">
@@ -7175,9 +7099,7 @@
       <c r="AR37" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="BH37" s="7" t="s">
-        <v>812</v>
-      </c>
+      <c r="BH37" s="2"/>
     </row>
     <row r="38" spans="1:60" ht="84" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
@@ -7309,9 +7231,7 @@
       <c r="BG38" s="4" t="s">
         <v>578</v>
       </c>
-      <c r="BH38" s="7" t="s">
-        <v>812</v>
-      </c>
+      <c r="BH38" s="2"/>
     </row>
     <row r="39" spans="1:60" ht="117.6" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
@@ -7404,9 +7324,7 @@
       <c r="BD39" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="BH39" s="7" t="s">
-        <v>812</v>
-      </c>
+      <c r="BH39" s="2"/>
     </row>
     <row r="40" spans="1:60" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">

</xml_diff>